<commit_message>
[V&V] Correções gerais no processo genérico de V&V
Correções nos templates de V&V e adição do template "Registro de
Anomalia"
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Genérico/6-Verificacao e Validacao/PLA-Planilha de Avaliação-VER-VAL.xlsx
+++ b/Artefatos de Documentação/Processo Genérico/6-Verificacao e Validacao/PLA-Planilha de Avaliação-VER-VAL.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="70">
   <si>
     <t>Projeto 1</t>
   </si>
@@ -94,9 +94,6 @@
     <t>PVV- Processo de VER/VAL&gt; Seção 5</t>
   </si>
   <si>
-    <t>PVVS - Plano de Verificação e Validação de Software &gt; Seção 4.5</t>
-  </si>
-  <si>
     <t>PVV- Processo de VER/VAL&gt; Seção 4</t>
   </si>
   <si>
@@ -106,58 +103,22 @@
     <t>PVVS - Plano de Verificação e Validação de Software&gt; Seção 6</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>OK (falta o cronograma)</t>
-  </si>
-  <si>
-    <t>ok</t>
-  </si>
-  <si>
     <t>[ID] RAN - [ID] Relato de Anomalia</t>
   </si>
   <si>
-    <t>Verificar com Gilmar</t>
-  </si>
-  <si>
     <t>PVV- Processo de VER/VAL&gt; Seções 4</t>
   </si>
   <si>
-    <t>PVVS - Plano de Verificação e Validação de Software&gt; Seções 2 e  4.4</t>
-  </si>
-  <si>
     <t>PVV- Processo de VER/VAL&gt; Seções 4 e 6</t>
   </si>
   <si>
-    <t>Gilmar</t>
-  </si>
-  <si>
-    <t>PT  - Plano de Teste&gt; Seção 2.1</t>
-  </si>
-  <si>
     <t>PT  - Plano de Teste&gt; Seções 2.6, 2.9 e 3.2</t>
   </si>
   <si>
-    <t>RT - Resultados de Teste&gt; Seções 3.1 e 3.3</t>
-  </si>
-  <si>
-    <t>PT - Plano de Teste&gt; Seção 4.3</t>
-  </si>
-  <si>
     <t>RT - Resultados de Teste</t>
   </si>
   <si>
-    <t>RT - Resultados de Teste &gt; Seções 3.1 e 3.3</t>
-  </si>
-  <si>
-    <t>PT - Plano de Teste&gt; Seção 3.6</t>
-  </si>
-  <si>
     <t>PT - Plano de Teste&gt; Seção 2.1</t>
-  </si>
-  <si>
-    <t>PT - Plano de Teste&gt; Seções 2.6, 2.9 e 3.2</t>
   </si>
   <si>
     <t>CT - Casos de Teste</t>
@@ -294,9 +255,6 @@
       </rPr>
       <t>As evidências apresentadas para este resultado permitem assegurar: (i) que foi definida uma política organizacional estabelecendo as expectativas da organização para a execução do processo e que esta política é conhecida e de fácil acesso aos interessados? (ii) que a política organizacional foi atualizada, quando necessário? (iii) que a política organizacional tem respaldo da alta administração (por exemplo, por meio de aprovação da alta administração)?</t>
     </r>
-  </si>
-  <si>
-    <t>PVVS - Plano de Verificação e Validação de Software&gt; Seção 9</t>
   </si>
   <si>
     <r>
@@ -383,28 +341,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">RAP 8. A comunicação entre as partes interessadas no processo é planejada e executada de forma a garantir o seu envolvimento.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">As evidências apresentadas para este resultado permitem assegurar que: (i) foi planejada a comunicação entre as partes interessadas no processo?; (ii) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>este planejamento foi monitorado?; (iii) existe evidência de que a comunicação ocorre de forma a garantir o envolvimento das partes interessadas?</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">RAP 9. (A partir do nível E). Métodos adequados para monitorar a eficácia e adequação do processo são determinados e os resultados do processo são revistos com a gerência de alto nível para fornecer visibilidade sobre a sua situação na organização.                                                                           
 </t>
     </r>
@@ -430,9 +366,6 @@
     </r>
   </si>
   <si>
-    <t>PVVS - Plano de Verificação e Validação de Software&gt; Seção 9.3</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">VER 1. Produtos de trabalho a serem verificados são identificados.
 </t>
@@ -515,6 +448,60 @@
   </si>
   <si>
     <t>PVVS - Plano de Verificação e Validação de Software&gt; Seção 8.2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RAP 8. A comunicação entre as partes interessadas no processo é planejada e executada de forma a garantir o seu envolvimento.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>As evidências apresentadas para este resultado permitem assegurar que: (i) foi planejada a comunicação entre as partes interessadas no processo?; (ii)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> este planejamento foi monitorado?; (iii) existe evidência de que a comunicação ocorre de forma a garantir o envolvimento das partes interessadas?</t>
+    </r>
+  </si>
+  <si>
+    <t>PT - Plano de Teste&gt; Seção 3.4</t>
+  </si>
+  <si>
+    <t>RT - Resultados de Teste&gt; Seção 3</t>
+  </si>
+  <si>
+    <t>Casos de Teste</t>
+  </si>
+  <si>
+    <t>RGA - Registro de Anomalias</t>
+  </si>
+  <si>
+    <t>PVVS - Plano de Verificação e Validação de Software&gt; Seções 2, 4.4 e 4.5</t>
+  </si>
+  <si>
+    <t>PVVS - Plano de Verificação e Validação de Software&gt; Seção 4.5</t>
+  </si>
+  <si>
+    <t>PT - Plano de Teste&gt; Seções 3.3</t>
+  </si>
+  <si>
+    <t>PVV- Processo de VER/VAL&gt; Seções 6</t>
+  </si>
+  <si>
+    <t>[ID] RAN - [ID] Relato de Anomalia (Linha "Comunicação")</t>
+  </si>
+  <si>
+    <t>RT - Resultados de Teste &gt; Seções 3</t>
+  </si>
+  <si>
+    <t>PT - Plano de Teste&gt; Seção 4.2</t>
   </si>
 </sst>
 </file>
@@ -967,7 +954,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1178,11 +1165,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="distributed"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1190,6 +1172,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="distributed" textRotation="180"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1601,10 +1586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H121"/>
+  <dimension ref="A1:H120"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="I116" sqref="I116"/>
+    <sheetView showGridLines="0" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -1622,7 +1607,7 @@
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="60"/>
-      <c r="D1" s="7"/>
+      <c r="D1" s="60"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -1634,7 +1619,7 @@
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="61"/>
-      <c r="D2" s="12"/>
+      <c r="D2" s="61"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -1650,7 +1635,7 @@
       <c r="C3" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="79" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="15" t="s">
@@ -1672,7 +1657,7 @@
       </c>
       <c r="B4" s="50"/>
       <c r="C4" s="62"/>
-      <c r="D4" s="49"/>
+      <c r="D4" s="62"/>
       <c r="E4" s="49"/>
       <c r="F4" s="49"/>
       <c r="G4" s="49"/>
@@ -1680,13 +1665,11 @@
     </row>
     <row r="5" spans="1:8" ht="38.25">
       <c r="A5" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="48" t="s">
-        <v>30</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B5" s="48"/>
       <c r="C5" s="63"/>
-      <c r="D5" s="48"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="48"/>
       <c r="F5" s="48"/>
       <c r="G5" s="48"/>
@@ -1700,7 +1683,7 @@
       <c r="C6" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="58"/>
+      <c r="D6" s="73"/>
       <c r="E6" s="58"/>
       <c r="F6" s="58"/>
       <c r="G6" s="58"/>
@@ -1708,13 +1691,13 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="74" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B7" s="59"/>
       <c r="C7" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="58"/>
+      <c r="D7" s="75"/>
       <c r="E7" s="58"/>
       <c r="F7" s="58"/>
       <c r="G7" s="58"/>
@@ -1724,7 +1707,7 @@
       <c r="A8" s="52"/>
       <c r="B8" s="59"/>
       <c r="C8" s="66"/>
-      <c r="D8" s="58"/>
+      <c r="D8" s="66"/>
       <c r="E8" s="58"/>
       <c r="F8" s="58"/>
       <c r="G8" s="58"/>
@@ -1734,7 +1717,7 @@
       <c r="A9" s="52"/>
       <c r="B9" s="59"/>
       <c r="C9" s="66"/>
-      <c r="D9" s="58"/>
+      <c r="D9" s="66"/>
       <c r="E9" s="58"/>
       <c r="F9" s="58"/>
       <c r="G9" s="58"/>
@@ -1744,7 +1727,7 @@
       <c r="A10" s="52"/>
       <c r="B10" s="59"/>
       <c r="C10" s="66"/>
-      <c r="D10" s="58"/>
+      <c r="D10" s="66"/>
       <c r="E10" s="58"/>
       <c r="F10" s="58"/>
       <c r="G10" s="58"/>
@@ -1756,7 +1739,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="21"/>
-      <c r="D11" s="53"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="53"/>
       <c r="F11" s="53"/>
       <c r="G11" s="53"/>
@@ -1764,13 +1747,11 @@
     </row>
     <row r="12" spans="1:8" ht="51">
       <c r="A12" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="48" t="s">
-        <v>36</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B12" s="48"/>
       <c r="C12" s="67"/>
-      <c r="D12" s="48"/>
+      <c r="D12" s="67"/>
       <c r="E12" s="48"/>
       <c r="F12" s="48"/>
       <c r="G12" s="48"/>
@@ -1778,26 +1759,31 @@
     </row>
     <row r="13" spans="1:8" ht="15">
       <c r="A13" s="74" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="20"/>
+        <v>26</v>
+      </c>
+      <c r="B13" s="59"/>
       <c r="C13" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="55"/>
+      <c r="D13" s="73"/>
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
       <c r="G13" s="55"/>
       <c r="H13" s="55"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="B14" s="76"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
+      <c r="A14" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="59"/>
+      <c r="C14" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="75"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:8" ht="15">
       <c r="A15" s="56"/>
@@ -1843,13 +1829,11 @@
     </row>
     <row r="19" spans="1:8" ht="51">
       <c r="A19" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>30</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B19" s="48"/>
       <c r="C19" s="67"/>
-      <c r="D19" s="48"/>
+      <c r="D19" s="67"/>
       <c r="E19" s="48"/>
       <c r="F19" s="48"/>
       <c r="G19" s="48"/>
@@ -1857,7 +1841,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="74" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B20" s="59"/>
       <c r="C20" s="75" t="s">
@@ -1873,7 +1857,7 @@
       <c r="A21" s="74"/>
       <c r="B21" s="59"/>
       <c r="C21" s="75"/>
-      <c r="D21" s="58"/>
+      <c r="D21" s="75"/>
       <c r="E21" s="58"/>
       <c r="F21" s="58"/>
       <c r="G21" s="58"/>
@@ -1923,13 +1907,11 @@
     </row>
     <row r="26" spans="1:8" ht="38.25">
       <c r="A26" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="48" t="s">
-        <v>36</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B26" s="48"/>
       <c r="C26" s="67"/>
-      <c r="D26" s="48"/>
+      <c r="D26" s="67"/>
       <c r="E26" s="48"/>
       <c r="F26" s="48"/>
       <c r="G26" s="48"/>
@@ -1937,13 +1919,13 @@
     </row>
     <row r="27" spans="1:8" ht="15">
       <c r="A27" s="74" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="B27" s="20"/>
-      <c r="C27" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="55"/>
+      <c r="C27" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="76"/>
       <c r="E27" s="55"/>
       <c r="F27" s="55"/>
       <c r="G27" s="55"/>
@@ -1951,13 +1933,13 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="74" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="B28" s="59"/>
       <c r="C28" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="58"/>
+      <c r="D28" s="75"/>
       <c r="E28" s="58"/>
       <c r="F28" s="58"/>
       <c r="G28" s="58"/>
@@ -1967,7 +1949,7 @@
       <c r="A29" s="74"/>
       <c r="B29" s="59"/>
       <c r="C29" s="75"/>
-      <c r="D29" s="58"/>
+      <c r="D29" s="75"/>
       <c r="E29" s="58"/>
       <c r="F29" s="58"/>
       <c r="G29" s="58"/>
@@ -1977,7 +1959,7 @@
       <c r="A30" s="56"/>
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
-      <c r="D30" s="55"/>
+      <c r="D30" s="20"/>
       <c r="E30" s="55"/>
       <c r="F30" s="55"/>
       <c r="G30" s="55"/>
@@ -1987,7 +1969,7 @@
       <c r="A31" s="54"/>
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
-      <c r="D31" s="55"/>
+      <c r="D31" s="20"/>
       <c r="E31" s="55"/>
       <c r="F31" s="55"/>
       <c r="G31" s="55"/>
@@ -2007,13 +1989,11 @@
     </row>
     <row r="33" spans="1:8" ht="40.5" customHeight="1">
       <c r="A33" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="48" t="s">
-        <v>30</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B33" s="48"/>
       <c r="C33" s="67"/>
-      <c r="D33" s="48"/>
+      <c r="D33" s="67"/>
       <c r="E33" s="48"/>
       <c r="F33" s="48"/>
       <c r="G33" s="48"/>
@@ -2021,43 +2001,51 @@
     </row>
     <row r="34" spans="1:8" ht="15">
       <c r="A34" s="74" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B34" s="20"/>
-      <c r="C34" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="55"/>
+      <c r="C34" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="76"/>
       <c r="E34" s="55"/>
       <c r="F34" s="55"/>
       <c r="G34" s="55"/>
       <c r="H34" s="55"/>
     </row>
-    <row r="35" spans="1:8" ht="15">
-      <c r="A35" s="74"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="79"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-    </row>
-    <row r="36" spans="1:8" ht="15">
-      <c r="A36" s="56"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
+    <row r="35" spans="1:8">
+      <c r="A35" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="18"/>
+      <c r="C35" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="76"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="59"/>
+      <c r="C36" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="75"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
     </row>
     <row r="37" spans="1:8" ht="15">
-      <c r="A37" s="56"/>
+      <c r="A37" s="74"/>
       <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="55"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="76"/>
       <c r="E37" s="55"/>
       <c r="F37" s="55"/>
       <c r="G37" s="55"/>
@@ -2065,89 +2053,85 @@
     </row>
     <row r="38" spans="1:8" ht="15">
       <c r="A38" s="54"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-    </row>
-    <row r="39" spans="1:8" ht="15">
-      <c r="A39" s="54"/>
-      <c r="B39" s="20" t="s">
+      <c r="B38" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="53"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="53"/>
-    </row>
-    <row r="40" spans="1:8" ht="38.25">
-      <c r="A40" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="48"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+    </row>
+    <row r="39" spans="1:8" ht="38.25">
+      <c r="A39" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="48"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
+    </row>
+    <row r="40" spans="1:8" ht="15">
+      <c r="A40" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="76"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="55"/>
     </row>
     <row r="41" spans="1:8" ht="15">
       <c r="A41" s="74" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B41" s="20"/>
-      <c r="C41" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="55"/>
+      <c r="C41" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="76"/>
       <c r="E41" s="55"/>
       <c r="F41" s="55"/>
       <c r="G41" s="55"/>
       <c r="H41" s="55"/>
     </row>
-    <row r="42" spans="1:8" ht="15">
+    <row r="42" spans="1:8">
       <c r="A42" s="74" t="s">
-        <v>20</v>
-      </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="55"/>
-      <c r="E42" s="55"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="55"/>
+        <v>25</v>
+      </c>
+      <c r="B42" s="18"/>
+      <c r="C42" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="76"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="74" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
+      <c r="A43" s="74"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
     </row>
     <row r="44" spans="1:8" ht="15">
-      <c r="A44" s="74" t="s">
-        <v>46</v>
-      </c>
+      <c r="A44" s="54"/>
       <c r="B44" s="20"/>
-      <c r="C44" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D44" s="55"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
       <c r="E44" s="55"/>
       <c r="F44" s="55"/>
       <c r="G44" s="55"/>
@@ -2155,105 +2139,103 @@
     </row>
     <row r="45" spans="1:8" ht="15">
       <c r="A45" s="54"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="55"/>
-    </row>
-    <row r="46" spans="1:8" ht="15">
-      <c r="A46" s="54"/>
-      <c r="B46" s="20" t="s">
+      <c r="B45" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-    </row>
-    <row r="47" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A47" s="24"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="68"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-    </row>
-    <row r="48" spans="1:8" ht="15.75">
-      <c r="A48" s="26" t="s">
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+    </row>
+    <row r="46" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A46" s="24"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="68"/>
+      <c r="D46" s="68"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="25"/>
+    </row>
+    <row r="47" spans="1:8" ht="15.75">
+      <c r="A47" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="27"/>
-      <c r="C48" s="69"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="29"/>
-    </row>
-    <row r="49" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A49" s="2" t="s">
+      <c r="B47" s="27"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="29"/>
+    </row>
+    <row r="48" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A48" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="30"/>
-      <c r="C49" s="70"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="33"/>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="3" t="s">
+      <c r="B48" s="30"/>
+      <c r="C48" s="70"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="33"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="34"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-    </row>
-    <row r="51" spans="1:8" ht="38.25">
-      <c r="A51" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="39"/>
-    </row>
-    <row r="52" spans="1:8" ht="15">
-      <c r="A52" s="74" t="s">
+      <c r="B49" s="34"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
+    </row>
+    <row r="50" spans="1:8" ht="38.25">
+      <c r="A50" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="37"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="39"/>
+    </row>
+    <row r="51" spans="1:8" ht="15">
+      <c r="A51" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="B52" s="20"/>
-      <c r="C52" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" s="55"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
-      <c r="G52" s="55"/>
-      <c r="H52" s="55"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="76"/>
+      <c r="E51" s="55"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="55"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="19"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="71"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="19"/>
       <c r="B53" s="18"/>
       <c r="C53" s="71"/>
-      <c r="D53" s="18"/>
+      <c r="D53" s="71"/>
       <c r="E53" s="18"/>
       <c r="F53" s="18"/>
       <c r="G53" s="18"/>
@@ -2263,7 +2245,7 @@
       <c r="A54" s="19"/>
       <c r="B54" s="18"/>
       <c r="C54" s="71"/>
-      <c r="D54" s="18"/>
+      <c r="D54" s="71"/>
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
@@ -2273,7 +2255,7 @@
       <c r="A55" s="19"/>
       <c r="B55" s="18"/>
       <c r="C55" s="71"/>
-      <c r="D55" s="18"/>
+      <c r="D55" s="71"/>
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
       <c r="G55" s="18"/>
@@ -2281,85 +2263,83 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="19"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="71"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="19"/>
-      <c r="B57" s="20" t="s">
+      <c r="B56" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="22"/>
-      <c r="H57" s="23"/>
-    </row>
-    <row r="58" spans="1:8" ht="15.75">
-      <c r="A58" s="40" t="s">
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="23"/>
+    </row>
+    <row r="57" spans="1:8" ht="15.75">
+      <c r="A57" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B58" s="41"/>
-      <c r="C58" s="72"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="42"/>
-      <c r="F58" s="42"/>
+      <c r="B57" s="41"/>
+      <c r="C57" s="72"/>
+      <c r="D57" s="72"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="39"/>
+    </row>
+    <row r="58" spans="1:8" ht="63.75">
+      <c r="A58" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="44"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="45"/>
       <c r="G58" s="39"/>
       <c r="H58" s="39"/>
     </row>
-    <row r="59" spans="1:8" ht="63.75">
-      <c r="A59" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="B59" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="45"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="39"/>
-    </row>
-    <row r="60" spans="1:8" ht="15">
+    <row r="59" spans="1:8" ht="15">
+      <c r="A59" s="74" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" s="20"/>
+      <c r="C59" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="76"/>
+      <c r="E59" s="55"/>
+      <c r="F59" s="55"/>
+      <c r="G59" s="55"/>
+      <c r="H59" s="55"/>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="74" t="s">
-        <v>22</v>
-      </c>
-      <c r="B60" s="20"/>
-      <c r="C60" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" s="55"/>
-      <c r="E60" s="55"/>
-      <c r="F60" s="55"/>
-      <c r="G60" s="55"/>
-      <c r="H60" s="55"/>
+        <v>56</v>
+      </c>
+      <c r="B60" s="59"/>
+      <c r="C60" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="73"/>
+      <c r="E60" s="58"/>
+      <c r="F60" s="58"/>
+      <c r="G60" s="58"/>
+      <c r="H60" s="58"/>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="74" t="s">
-        <v>72</v>
-      </c>
-      <c r="B61" s="59"/>
-      <c r="C61" s="73" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" s="58"/>
-      <c r="E61" s="58"/>
-      <c r="F61" s="58"/>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58"/>
+      <c r="A61" s="19"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="71"/>
+      <c r="D61" s="71"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="19"/>
       <c r="B62" s="18"/>
       <c r="C62" s="71"/>
-      <c r="D62" s="18"/>
+      <c r="D62" s="71"/>
       <c r="E62" s="18"/>
       <c r="F62" s="18"/>
       <c r="G62" s="18"/>
@@ -2369,7 +2349,7 @@
       <c r="A63" s="19"/>
       <c r="B63" s="18"/>
       <c r="C63" s="71"/>
-      <c r="D63" s="18"/>
+      <c r="D63" s="71"/>
       <c r="E63" s="18"/>
       <c r="F63" s="18"/>
       <c r="G63" s="18"/>
@@ -2377,59 +2357,57 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="19"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="71"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="18"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18"/>
-      <c r="H64" s="18"/>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="19"/>
-      <c r="B65" s="20" t="s">
+      <c r="B64" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
-      <c r="E65" s="21"/>
-      <c r="F65" s="21"/>
-      <c r="G65" s="22"/>
-      <c r="H65" s="23"/>
-    </row>
-    <row r="66" spans="1:8" ht="26.25">
-      <c r="A66" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="B66" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="C66" s="72"/>
-      <c r="D66" s="47"/>
-      <c r="E66" s="47"/>
-      <c r="F66" s="47"/>
-      <c r="G66" s="39"/>
-      <c r="H66" s="39"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="23"/>
+    </row>
+    <row r="65" spans="1:8" ht="26.25">
+      <c r="A65" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B65" s="46"/>
+      <c r="C65" s="72"/>
+      <c r="D65" s="72"/>
+      <c r="E65" s="47"/>
+      <c r="F65" s="47"/>
+      <c r="G65" s="39"/>
+      <c r="H65" s="39"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="74" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="59"/>
+      <c r="C66" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="73"/>
+      <c r="E66" s="58"/>
+      <c r="F66" s="58"/>
+      <c r="G66" s="58"/>
+      <c r="H66" s="58"/>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="74" t="s">
-        <v>19</v>
-      </c>
-      <c r="B67" s="59"/>
-      <c r="C67" s="73" t="s">
-        <v>17</v>
-      </c>
-      <c r="D67" s="58"/>
-      <c r="E67" s="58"/>
-      <c r="F67" s="58"/>
-      <c r="G67" s="58"/>
-      <c r="H67" s="58"/>
+      <c r="A67" s="19"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="71"/>
+      <c r="D67" s="71"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="19"/>
       <c r="B68" s="18"/>
       <c r="C68" s="71"/>
-      <c r="D68" s="18"/>
+      <c r="D68" s="71"/>
       <c r="E68" s="18"/>
       <c r="F68" s="18"/>
       <c r="G68" s="18"/>
@@ -2439,7 +2417,7 @@
       <c r="A69" s="19"/>
       <c r="B69" s="18"/>
       <c r="C69" s="71"/>
-      <c r="D69" s="18"/>
+      <c r="D69" s="71"/>
       <c r="E69" s="18"/>
       <c r="F69" s="18"/>
       <c r="G69" s="18"/>
@@ -2449,7 +2427,7 @@
       <c r="A70" s="19"/>
       <c r="B70" s="18"/>
       <c r="C70" s="71"/>
-      <c r="D70" s="18"/>
+      <c r="D70" s="71"/>
       <c r="E70" s="18"/>
       <c r="F70" s="18"/>
       <c r="G70" s="18"/>
@@ -2457,73 +2435,79 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="19"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="71"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="18"/>
-      <c r="H71" s="18"/>
-    </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="19"/>
-      <c r="B72" s="20" t="s">
+      <c r="B71" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C72" s="21"/>
-      <c r="D72" s="21"/>
-      <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
-      <c r="G72" s="22"/>
-      <c r="H72" s="23"/>
-    </row>
-    <row r="73" spans="1:8" ht="51.75">
-      <c r="A73" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="B73" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="C73" s="72"/>
-      <c r="D73" s="47"/>
-      <c r="E73" s="47"/>
-      <c r="F73" s="47"/>
-      <c r="G73" s="39"/>
-      <c r="H73" s="39"/>
-    </row>
-    <row r="74" spans="1:8" ht="15">
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="22"/>
+      <c r="H71" s="23"/>
+    </row>
+    <row r="72" spans="1:8" ht="51.75">
+      <c r="A72" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B72" s="47"/>
+      <c r="C72" s="72"/>
+      <c r="D72" s="72"/>
+      <c r="E72" s="47"/>
+      <c r="F72" s="47"/>
+      <c r="G72" s="39"/>
+      <c r="H72" s="39"/>
+    </row>
+    <row r="73" spans="1:8" ht="15">
+      <c r="A73" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" s="20"/>
+      <c r="C73" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="76"/>
+      <c r="E73" s="55"/>
+      <c r="F73" s="55"/>
+      <c r="G73" s="55"/>
+      <c r="H73" s="55"/>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="B74" s="20"/>
-      <c r="C74" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D74" s="55"/>
-      <c r="E74" s="55"/>
-      <c r="F74" s="55"/>
-      <c r="G74" s="55"/>
-      <c r="H74" s="55"/>
-    </row>
-    <row r="75" spans="1:8">
+        <v>57</v>
+      </c>
+      <c r="B74" s="59"/>
+      <c r="C74" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="D74" s="73"/>
+      <c r="E74" s="58"/>
+      <c r="F74" s="58"/>
+      <c r="G74" s="58"/>
+      <c r="H74" s="58"/>
+    </row>
+    <row r="75" spans="1:8" ht="15">
       <c r="A75" s="74" t="s">
-        <v>73</v>
-      </c>
-      <c r="B75" s="59"/>
-      <c r="C75" s="73" t="s">
-        <v>17</v>
-      </c>
-      <c r="D75" s="58"/>
-      <c r="E75" s="58"/>
-      <c r="F75" s="58"/>
-      <c r="G75" s="58"/>
-      <c r="H75" s="58"/>
+        <v>31</v>
+      </c>
+      <c r="B75" s="20"/>
+      <c r="C75" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="76"/>
+      <c r="E75" s="55"/>
+      <c r="F75" s="55"/>
+      <c r="G75" s="55"/>
+      <c r="H75" s="55"/>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="19"/>
+      <c r="A76" s="74" t="s">
+        <v>62</v>
+      </c>
       <c r="B76" s="18"/>
-      <c r="C76" s="71"/>
-      <c r="D76" s="18"/>
+      <c r="C76" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D76" s="76"/>
       <c r="E76" s="18"/>
       <c r="F76" s="18"/>
       <c r="G76" s="18"/>
@@ -2533,7 +2517,7 @@
       <c r="A77" s="19"/>
       <c r="B77" s="18"/>
       <c r="C77" s="71"/>
-      <c r="D77" s="18"/>
+      <c r="D77" s="71"/>
       <c r="E77" s="18"/>
       <c r="F77" s="18"/>
       <c r="G77" s="18"/>
@@ -2541,73 +2525,71 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="19"/>
-      <c r="B78" s="18"/>
-      <c r="C78" s="71"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="18"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="18"/>
-      <c r="H78" s="18"/>
-    </row>
-    <row r="79" spans="1:8">
-      <c r="A79" s="19"/>
-      <c r="B79" s="20" t="s">
+      <c r="B78" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="21"/>
-      <c r="G79" s="22"/>
-      <c r="H79" s="23"/>
-    </row>
-    <row r="80" spans="1:8" ht="64.5">
-      <c r="A80" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="B80" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C80" s="72"/>
-      <c r="D80" s="47"/>
-      <c r="E80" s="47"/>
-      <c r="F80" s="47"/>
-      <c r="G80" s="39"/>
-      <c r="H80" s="39"/>
-    </row>
-    <row r="81" spans="1:8">
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="22"/>
+      <c r="H78" s="23"/>
+    </row>
+    <row r="79" spans="1:8" ht="64.5">
+      <c r="A79" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B79" s="37"/>
+      <c r="C79" s="72"/>
+      <c r="D79" s="72"/>
+      <c r="E79" s="47"/>
+      <c r="F79" s="47"/>
+      <c r="G79" s="39"/>
+      <c r="H79" s="39"/>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="74" t="s">
+        <v>63</v>
+      </c>
+      <c r="B80" s="59"/>
+      <c r="C80" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="D80" s="73"/>
+      <c r="E80" s="58"/>
+      <c r="F80" s="58"/>
+      <c r="G80" s="58"/>
+      <c r="H80" s="58"/>
+    </row>
+    <row r="81" spans="1:8" ht="15">
       <c r="A81" s="74" t="s">
-        <v>34</v>
-      </c>
-      <c r="B81" s="59"/>
-      <c r="C81" s="73" t="s">
-        <v>17</v>
-      </c>
-      <c r="D81" s="58"/>
-      <c r="E81" s="58"/>
-      <c r="F81" s="58"/>
-      <c r="G81" s="58"/>
-      <c r="H81" s="58"/>
-    </row>
-    <row r="82" spans="1:8" ht="15">
-      <c r="A82" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="B82" s="20"/>
-      <c r="C82" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D82" s="55"/>
-      <c r="E82" s="55"/>
-      <c r="F82" s="55"/>
-      <c r="G82" s="55"/>
-      <c r="H82" s="55"/>
+        <v>24</v>
+      </c>
+      <c r="B81" s="20"/>
+      <c r="C81" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D81" s="76"/>
+      <c r="E81" s="55"/>
+      <c r="F81" s="55"/>
+      <c r="G81" s="55"/>
+      <c r="H81" s="55"/>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="19"/>
+      <c r="B82" s="18"/>
+      <c r="C82" s="71"/>
+      <c r="D82" s="71"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="19"/>
       <c r="B83" s="18"/>
       <c r="C83" s="71"/>
-      <c r="D83" s="18"/>
+      <c r="D83" s="71"/>
       <c r="E83" s="18"/>
       <c r="F83" s="18"/>
       <c r="G83" s="18"/>
@@ -2617,7 +2599,7 @@
       <c r="A84" s="19"/>
       <c r="B84" s="18"/>
       <c r="C84" s="71"/>
-      <c r="D84" s="18"/>
+      <c r="D84" s="71"/>
       <c r="E84" s="18"/>
       <c r="F84" s="18"/>
       <c r="G84" s="18"/>
@@ -2625,73 +2607,71 @@
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="19"/>
-      <c r="B85" s="18"/>
-      <c r="C85" s="71"/>
-      <c r="D85" s="18"/>
-      <c r="E85" s="18"/>
-      <c r="F85" s="18"/>
-      <c r="G85" s="18"/>
-      <c r="H85" s="18"/>
-    </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="19"/>
-      <c r="B86" s="20" t="s">
+      <c r="B85" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C86" s="21"/>
-      <c r="D86" s="21"/>
-      <c r="E86" s="21"/>
-      <c r="F86" s="21"/>
-      <c r="G86" s="22"/>
-      <c r="H86" s="23"/>
-    </row>
-    <row r="87" spans="1:8" ht="51.75">
-      <c r="A87" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="B87" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="C87" s="72"/>
-      <c r="D87" s="47"/>
-      <c r="E87" s="47"/>
-      <c r="F87" s="47"/>
-      <c r="G87" s="39"/>
-      <c r="H87" s="39"/>
-    </row>
-    <row r="88" spans="1:8" ht="15">
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="22"/>
+      <c r="H85" s="23"/>
+    </row>
+    <row r="86" spans="1:8" ht="51.75">
+      <c r="A86" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B86" s="47"/>
+      <c r="C86" s="72"/>
+      <c r="D86" s="72"/>
+      <c r="E86" s="47"/>
+      <c r="F86" s="47"/>
+      <c r="G86" s="39"/>
+      <c r="H86" s="39"/>
+    </row>
+    <row r="87" spans="1:8" ht="15">
+      <c r="A87" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="B87" s="20"/>
+      <c r="C87" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D87" s="76"/>
+      <c r="E87" s="55"/>
+      <c r="F87" s="55"/>
+      <c r="G87" s="55"/>
+      <c r="H87" s="55"/>
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" s="74" t="s">
-        <v>35</v>
-      </c>
-      <c r="B88" s="20"/>
-      <c r="C88" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D88" s="55"/>
-      <c r="E88" s="55"/>
-      <c r="F88" s="55"/>
-      <c r="G88" s="55"/>
-      <c r="H88" s="55"/>
+        <v>64</v>
+      </c>
+      <c r="B88" s="59"/>
+      <c r="C88" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="D88" s="73"/>
+      <c r="E88" s="58"/>
+      <c r="F88" s="58"/>
+      <c r="G88" s="58"/>
+      <c r="H88" s="58"/>
     </row>
     <row r="89" spans="1:8">
-      <c r="A89" s="74" t="s">
-        <v>24</v>
-      </c>
-      <c r="B89" s="59"/>
-      <c r="C89" s="73" t="s">
-        <v>17</v>
-      </c>
-      <c r="D89" s="58"/>
-      <c r="E89" s="58"/>
-      <c r="F89" s="58"/>
-      <c r="G89" s="58"/>
-      <c r="H89" s="58"/>
+      <c r="A89" s="19"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="71"/>
+      <c r="D89" s="71"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="18"/>
+      <c r="G89" s="18"/>
+      <c r="H89" s="18"/>
     </row>
     <row r="90" spans="1:8">
       <c r="A90" s="19"/>
       <c r="B90" s="18"/>
       <c r="C90" s="71"/>
-      <c r="D90" s="18"/>
+      <c r="D90" s="71"/>
       <c r="E90" s="18"/>
       <c r="F90" s="18"/>
       <c r="G90" s="18"/>
@@ -2701,7 +2681,7 @@
       <c r="A91" s="19"/>
       <c r="B91" s="18"/>
       <c r="C91" s="71"/>
-      <c r="D91" s="18"/>
+      <c r="D91" s="71"/>
       <c r="E91" s="18"/>
       <c r="F91" s="18"/>
       <c r="G91" s="18"/>
@@ -2709,73 +2689,71 @@
     </row>
     <row r="92" spans="1:8">
       <c r="A92" s="19"/>
-      <c r="B92" s="18"/>
-      <c r="C92" s="71"/>
-      <c r="D92" s="18"/>
-      <c r="E92" s="18"/>
-      <c r="F92" s="18"/>
-      <c r="G92" s="18"/>
-      <c r="H92" s="18"/>
-    </row>
-    <row r="93" spans="1:8">
-      <c r="A93" s="19"/>
-      <c r="B93" s="20" t="s">
+      <c r="B92" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C93" s="21"/>
-      <c r="D93" s="21"/>
-      <c r="E93" s="21"/>
-      <c r="F93" s="21"/>
-      <c r="G93" s="22"/>
-      <c r="H93" s="23"/>
-    </row>
-    <row r="94" spans="1:8" ht="64.5">
-      <c r="A94" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="B94" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C94" s="72"/>
-      <c r="D94" s="47"/>
-      <c r="E94" s="47"/>
-      <c r="F94" s="47"/>
-      <c r="G94" s="39"/>
-      <c r="H94" s="39"/>
-    </row>
-    <row r="95" spans="1:8" ht="15">
+      <c r="C92" s="21"/>
+      <c r="D92" s="21"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="21"/>
+      <c r="G92" s="22"/>
+      <c r="H92" s="23"/>
+    </row>
+    <row r="93" spans="1:8" ht="64.5">
+      <c r="A93" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B93" s="37"/>
+      <c r="C93" s="72"/>
+      <c r="D93" s="72"/>
+      <c r="E93" s="47"/>
+      <c r="F93" s="47"/>
+      <c r="G93" s="39"/>
+      <c r="H93" s="39"/>
+    </row>
+    <row r="94" spans="1:8" ht="15">
+      <c r="A94" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="B94" s="20"/>
+      <c r="C94" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D94" s="76"/>
+      <c r="E94" s="55"/>
+      <c r="F94" s="55"/>
+      <c r="G94" s="55"/>
+      <c r="H94" s="55"/>
+    </row>
+    <row r="95" spans="1:8">
       <c r="A95" s="74" t="s">
-        <v>25</v>
-      </c>
-      <c r="B95" s="20"/>
-      <c r="C95" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D95" s="55"/>
-      <c r="E95" s="55"/>
-      <c r="F95" s="55"/>
-      <c r="G95" s="55"/>
-      <c r="H95" s="55"/>
+        <v>65</v>
+      </c>
+      <c r="B95" s="59"/>
+      <c r="C95" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="D95" s="75"/>
+      <c r="E95" s="58"/>
+      <c r="F95" s="58"/>
+      <c r="G95" s="58"/>
+      <c r="H95" s="58"/>
     </row>
     <row r="96" spans="1:8">
-      <c r="A96" s="74" t="s">
-        <v>43</v>
-      </c>
-      <c r="B96" s="59"/>
-      <c r="C96" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="D96" s="58"/>
-      <c r="E96" s="58"/>
-      <c r="F96" s="58"/>
-      <c r="G96" s="58"/>
-      <c r="H96" s="58"/>
+      <c r="A96" s="19"/>
+      <c r="B96" s="18"/>
+      <c r="C96" s="71"/>
+      <c r="D96" s="71"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="18"/>
+      <c r="G96" s="18"/>
+      <c r="H96" s="18"/>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" s="19"/>
       <c r="B97" s="18"/>
       <c r="C97" s="71"/>
-      <c r="D97" s="18"/>
+      <c r="D97" s="71"/>
       <c r="E97" s="18"/>
       <c r="F97" s="18"/>
       <c r="G97" s="18"/>
@@ -2785,7 +2763,7 @@
       <c r="A98" s="19"/>
       <c r="B98" s="18"/>
       <c r="C98" s="71"/>
-      <c r="D98" s="18"/>
+      <c r="D98" s="71"/>
       <c r="E98" s="18"/>
       <c r="F98" s="18"/>
       <c r="G98" s="18"/>
@@ -2793,49 +2771,51 @@
     </row>
     <row r="99" spans="1:8">
       <c r="A99" s="19"/>
-      <c r="B99" s="18"/>
-      <c r="C99" s="71"/>
-      <c r="D99" s="18"/>
-      <c r="E99" s="18"/>
-      <c r="F99" s="18"/>
-      <c r="G99" s="18"/>
-      <c r="H99" s="18"/>
-    </row>
-    <row r="100" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A100" s="19"/>
-      <c r="B100" s="20" t="s">
+      <c r="B99" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C100" s="21"/>
-      <c r="D100" s="21"/>
-      <c r="E100" s="21"/>
-      <c r="F100" s="21"/>
-      <c r="G100" s="22"/>
-      <c r="H100" s="23"/>
-    </row>
-    <row r="101" spans="1:8" ht="69.75" customHeight="1">
-      <c r="A101" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="B101" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="C101" s="72"/>
-      <c r="D101" s="47"/>
-      <c r="E101" s="47"/>
-      <c r="F101" s="47"/>
-      <c r="G101" s="39"/>
-      <c r="H101" s="39"/>
+      <c r="C99" s="21"/>
+      <c r="D99" s="21"/>
+      <c r="E99" s="21"/>
+      <c r="F99" s="21"/>
+      <c r="G99" s="22"/>
+      <c r="H99" s="23"/>
+    </row>
+    <row r="100" spans="1:8" ht="64.5">
+      <c r="A100" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B100" s="37"/>
+      <c r="C100" s="72"/>
+      <c r="D100" s="72"/>
+      <c r="E100" s="47"/>
+      <c r="F100" s="47"/>
+      <c r="G100" s="39"/>
+      <c r="H100" s="39"/>
+    </row>
+    <row r="101" spans="1:8" ht="15">
+      <c r="A101" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="B101" s="20"/>
+      <c r="C101" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D101" s="76"/>
+      <c r="E101" s="55"/>
+      <c r="F101" s="55"/>
+      <c r="G101" s="55"/>
+      <c r="H101" s="55"/>
     </row>
     <row r="102" spans="1:8" ht="15">
       <c r="A102" s="74" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="B102" s="20"/>
-      <c r="C102" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D102" s="55"/>
+      <c r="C102" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D102" s="76"/>
       <c r="E102" s="55"/>
       <c r="F102" s="55"/>
       <c r="G102" s="55"/>
@@ -2845,7 +2825,7 @@
       <c r="A103" s="19"/>
       <c r="B103" s="18"/>
       <c r="C103" s="71"/>
-      <c r="D103" s="18"/>
+      <c r="D103" s="71"/>
       <c r="E103" s="18"/>
       <c r="F103" s="18"/>
       <c r="G103" s="18"/>
@@ -2855,7 +2835,7 @@
       <c r="A104" s="19"/>
       <c r="B104" s="18"/>
       <c r="C104" s="71"/>
-      <c r="D104" s="18"/>
+      <c r="D104" s="71"/>
       <c r="E104" s="18"/>
       <c r="F104" s="18"/>
       <c r="G104" s="18"/>
@@ -2865,7 +2845,7 @@
       <c r="A105" s="19"/>
       <c r="B105" s="18"/>
       <c r="C105" s="71"/>
-      <c r="D105" s="18"/>
+      <c r="D105" s="71"/>
       <c r="E105" s="18"/>
       <c r="F105" s="18"/>
       <c r="G105" s="18"/>
@@ -2873,59 +2853,65 @@
     </row>
     <row r="106" spans="1:8">
       <c r="A106" s="19"/>
-      <c r="B106" s="18"/>
-      <c r="C106" s="71"/>
-      <c r="D106" s="18"/>
-      <c r="E106" s="18"/>
-      <c r="F106" s="18"/>
-      <c r="G106" s="18"/>
-      <c r="H106" s="18"/>
-    </row>
-    <row r="107" spans="1:8">
-      <c r="A107" s="19"/>
-      <c r="B107" s="20" t="s">
+      <c r="B106" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C107" s="21"/>
-      <c r="D107" s="21"/>
-      <c r="E107" s="21"/>
-      <c r="F107" s="21"/>
-      <c r="G107" s="22"/>
-      <c r="H107" s="23"/>
-    </row>
-    <row r="108" spans="1:8" ht="64.5">
-      <c r="A108" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="B108" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="C108" s="72"/>
-      <c r="D108" s="47"/>
-      <c r="E108" s="47"/>
-      <c r="F108" s="47"/>
-      <c r="G108" s="39"/>
-      <c r="H108" s="39"/>
-    </row>
-    <row r="109" spans="1:8">
+      <c r="C106" s="21"/>
+      <c r="D106" s="21"/>
+      <c r="E106" s="21"/>
+      <c r="F106" s="21"/>
+      <c r="G106" s="22"/>
+      <c r="H106" s="23"/>
+    </row>
+    <row r="107" spans="1:8" ht="64.5">
+      <c r="A107" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B107" s="47"/>
+      <c r="C107" s="72"/>
+      <c r="D107" s="72"/>
+      <c r="E107" s="47"/>
+      <c r="F107" s="47"/>
+      <c r="G107" s="39"/>
+      <c r="H107" s="39"/>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="B108" s="18"/>
+      <c r="C108" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D108" s="76"/>
+      <c r="E108" s="18"/>
+      <c r="F108" s="18"/>
+      <c r="G108" s="18"/>
+      <c r="H108" s="18"/>
+    </row>
+    <row r="109" spans="1:8" ht="15">
       <c r="A109" s="74" t="s">
-        <v>26</v>
-      </c>
-      <c r="B109" s="18"/>
-      <c r="C109" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D109" s="18"/>
-      <c r="E109" s="18"/>
-      <c r="F109" s="18"/>
-      <c r="G109" s="18"/>
-      <c r="H109" s="18"/>
+        <v>31</v>
+      </c>
+      <c r="B109" s="20"/>
+      <c r="C109" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D109" s="76"/>
+      <c r="E109" s="55"/>
+      <c r="F109" s="55"/>
+      <c r="G109" s="55"/>
+      <c r="H109" s="55"/>
     </row>
     <row r="110" spans="1:8">
-      <c r="A110" s="19"/>
+      <c r="A110" s="74" t="s">
+        <v>62</v>
+      </c>
       <c r="B110" s="18"/>
-      <c r="C110" s="71"/>
-      <c r="D110" s="18"/>
+      <c r="C110" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D110" s="76"/>
       <c r="E110" s="18"/>
       <c r="F110" s="18"/>
       <c r="G110" s="18"/>
@@ -2935,7 +2921,7 @@
       <c r="A111" s="19"/>
       <c r="B111" s="18"/>
       <c r="C111" s="71"/>
-      <c r="D111" s="18"/>
+      <c r="D111" s="71"/>
       <c r="E111" s="18"/>
       <c r="F111" s="18"/>
       <c r="G111" s="18"/>
@@ -2945,7 +2931,7 @@
       <c r="A112" s="19"/>
       <c r="B112" s="18"/>
       <c r="C112" s="71"/>
-      <c r="D112" s="18"/>
+      <c r="D112" s="71"/>
       <c r="E112" s="18"/>
       <c r="F112" s="18"/>
       <c r="G112" s="18"/>
@@ -2953,77 +2939,79 @@
     </row>
     <row r="113" spans="1:8">
       <c r="A113" s="19"/>
-      <c r="B113" s="18"/>
-      <c r="C113" s="71"/>
-      <c r="D113" s="18"/>
-      <c r="E113" s="18"/>
-      <c r="F113" s="18"/>
-      <c r="G113" s="18"/>
-      <c r="H113" s="18"/>
-    </row>
-    <row r="114" spans="1:8">
-      <c r="A114" s="19"/>
-      <c r="B114" s="20" t="s">
+      <c r="B113" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C114" s="21"/>
-      <c r="D114" s="21"/>
-      <c r="E114" s="21"/>
-      <c r="F114" s="21"/>
-      <c r="G114" s="22"/>
-      <c r="H114" s="23"/>
-    </row>
-    <row r="115" spans="1:8" ht="64.5">
-      <c r="A115" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="B115" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="C115" s="72"/>
-      <c r="D115" s="47"/>
-      <c r="E115" s="47"/>
-      <c r="F115" s="47"/>
-      <c r="G115" s="39"/>
-      <c r="H115" s="39"/>
+      <c r="C113" s="21"/>
+      <c r="D113" s="21"/>
+      <c r="E113" s="21"/>
+      <c r="F113" s="21"/>
+      <c r="G113" s="22"/>
+      <c r="H113" s="23"/>
+    </row>
+    <row r="114" spans="1:8" ht="64.5">
+      <c r="A114" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B114" s="47"/>
+      <c r="C114" s="72"/>
+      <c r="D114" s="72"/>
+      <c r="E114" s="47"/>
+      <c r="F114" s="47"/>
+      <c r="G114" s="39"/>
+      <c r="H114" s="39"/>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" s="74" t="s">
+        <v>56</v>
+      </c>
+      <c r="B115" s="59"/>
+      <c r="C115" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="D115" s="73"/>
+      <c r="E115" s="58"/>
+      <c r="F115" s="58"/>
+      <c r="G115" s="58"/>
+      <c r="H115" s="58"/>
     </row>
     <row r="116" spans="1:8">
       <c r="A116" s="74" t="s">
-        <v>72</v>
-      </c>
-      <c r="B116" s="59"/>
-      <c r="C116" s="73" t="s">
-        <v>17</v>
-      </c>
-      <c r="D116" s="58"/>
-      <c r="E116" s="58"/>
-      <c r="F116" s="58"/>
-      <c r="G116" s="58"/>
-      <c r="H116" s="58"/>
-    </row>
-    <row r="117" spans="1:8">
+        <v>25</v>
+      </c>
+      <c r="B116" s="18"/>
+      <c r="C116" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D116" s="76"/>
+      <c r="E116" s="18"/>
+      <c r="F116" s="18"/>
+      <c r="G116" s="18"/>
+      <c r="H116" s="18"/>
+    </row>
+    <row r="117" spans="1:8" ht="15">
       <c r="A117" s="74" t="s">
-        <v>26</v>
-      </c>
-      <c r="B117" s="18"/>
-      <c r="C117" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D117" s="18"/>
-      <c r="E117" s="18"/>
-      <c r="F117" s="18"/>
-      <c r="G117" s="18"/>
-      <c r="H117" s="18"/>
+        <v>27</v>
+      </c>
+      <c r="B117" s="20"/>
+      <c r="C117" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D117" s="76"/>
+      <c r="E117" s="55"/>
+      <c r="F117" s="55"/>
+      <c r="G117" s="55"/>
+      <c r="H117" s="55"/>
     </row>
     <row r="118" spans="1:8">
       <c r="A118" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="B118" s="20"/>
-      <c r="C118" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D118" s="18"/>
+        <v>62</v>
+      </c>
+      <c r="B118" s="18"/>
+      <c r="C118" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D118" s="76"/>
       <c r="E118" s="18"/>
       <c r="F118" s="18"/>
       <c r="G118" s="18"/>
@@ -3033,7 +3021,7 @@
       <c r="A119" s="19"/>
       <c r="B119" s="18"/>
       <c r="C119" s="71"/>
-      <c r="D119" s="18"/>
+      <c r="D119" s="71"/>
       <c r="E119" s="18"/>
       <c r="F119" s="18"/>
       <c r="G119" s="18"/>
@@ -3041,60 +3029,58 @@
     </row>
     <row r="120" spans="1:8">
       <c r="A120" s="19"/>
-      <c r="B120" s="18"/>
-      <c r="C120" s="71"/>
-      <c r="D120" s="18"/>
-      <c r="E120" s="18"/>
-      <c r="F120" s="18"/>
-      <c r="G120" s="18"/>
-      <c r="H120" s="18"/>
-    </row>
-    <row r="121" spans="1:8">
-      <c r="A121" s="19"/>
-      <c r="B121" s="20" t="s">
+      <c r="B120" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C121" s="21"/>
-      <c r="D121" s="21"/>
-      <c r="E121" s="21"/>
-      <c r="F121" s="21"/>
-      <c r="G121" s="22"/>
-      <c r="H121" s="23"/>
+      <c r="C120" s="21"/>
+      <c r="D120" s="21"/>
+      <c r="E120" s="21"/>
+      <c r="F120" s="21"/>
+      <c r="G120" s="22"/>
+      <c r="H120" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
     <hyperlink ref="C7" r:id="rId2"/>
-    <hyperlink ref="C13" r:id="rId3"/>
-    <hyperlink ref="C20" r:id="rId4"/>
-    <hyperlink ref="C28" r:id="rId5"/>
-    <hyperlink ref="C27" r:id="rId6"/>
-    <hyperlink ref="C34" r:id="rId7"/>
-    <hyperlink ref="C41" r:id="rId8"/>
-    <hyperlink ref="C42" r:id="rId9"/>
-    <hyperlink ref="C43" r:id="rId10"/>
-    <hyperlink ref="C52" r:id="rId11"/>
-    <hyperlink ref="C60" r:id="rId12"/>
-    <hyperlink ref="C67" r:id="rId13"/>
-    <hyperlink ref="C74" r:id="rId14"/>
-    <hyperlink ref="C61" r:id="rId15"/>
-    <hyperlink ref="C75" r:id="rId16"/>
-    <hyperlink ref="C81" r:id="rId17"/>
-    <hyperlink ref="C82" r:id="rId18"/>
-    <hyperlink ref="C88" r:id="rId19"/>
-    <hyperlink ref="C89" r:id="rId20"/>
-    <hyperlink ref="C95" r:id="rId21"/>
-    <hyperlink ref="C96" r:id="rId22"/>
-    <hyperlink ref="C102" r:id="rId23"/>
-    <hyperlink ref="C109" r:id="rId24"/>
-    <hyperlink ref="C116" r:id="rId25"/>
-    <hyperlink ref="C117" r:id="rId26"/>
-    <hyperlink ref="C118" r:id="rId27"/>
-    <hyperlink ref="C44" r:id="rId28"/>
+    <hyperlink ref="C28" r:id="rId3"/>
+    <hyperlink ref="C27" r:id="rId4"/>
+    <hyperlink ref="C34" r:id="rId5"/>
+    <hyperlink ref="C41" r:id="rId6"/>
+    <hyperlink ref="C42" r:id="rId7"/>
+    <hyperlink ref="C36" r:id="rId8"/>
+    <hyperlink ref="C51" r:id="rId9"/>
+    <hyperlink ref="C102" r:id="rId10"/>
+    <hyperlink ref="C108" r:id="rId11"/>
+    <hyperlink ref="C117" r:id="rId12"/>
+    <hyperlink ref="C75" r:id="rId13"/>
+    <hyperlink ref="C76" r:id="rId14"/>
+    <hyperlink ref="C109" r:id="rId15"/>
+    <hyperlink ref="C110" r:id="rId16"/>
+    <hyperlink ref="C118" r:id="rId17"/>
+    <hyperlink ref="C35" r:id="rId18"/>
+    <hyperlink ref="C13" r:id="rId19"/>
+    <hyperlink ref="C60" r:id="rId20"/>
+    <hyperlink ref="C66" r:id="rId21"/>
+    <hyperlink ref="C74" r:id="rId22"/>
+    <hyperlink ref="C80" r:id="rId23"/>
+    <hyperlink ref="C88" r:id="rId24"/>
+    <hyperlink ref="C115" r:id="rId25"/>
+    <hyperlink ref="C14" r:id="rId26"/>
+    <hyperlink ref="C95" r:id="rId27"/>
+    <hyperlink ref="C40" r:id="rId28"/>
+    <hyperlink ref="C59" r:id="rId29"/>
+    <hyperlink ref="C73" r:id="rId30"/>
+    <hyperlink ref="C81" r:id="rId31"/>
+    <hyperlink ref="C87" r:id="rId32"/>
+    <hyperlink ref="C94" r:id="rId33"/>
+    <hyperlink ref="C101" r:id="rId34"/>
+    <hyperlink ref="C116" r:id="rId35"/>
+    <hyperlink ref="C20" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.49212598499999999" footer="0.49212598499999999"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -3104,7 +3090,7 @@
   <dimension ref="A1:H149"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3179,11 +3165,9 @@
     </row>
     <row r="5" spans="1:8" ht="38.25">
       <c r="A5" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="48" t="s">
-        <v>28</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
       <c r="E5" s="48"/>
@@ -3199,7 +3183,7 @@
       <c r="C6" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="58"/>
+      <c r="D6" s="73"/>
       <c r="E6" s="58"/>
       <c r="F6" s="58"/>
       <c r="G6" s="58"/>
@@ -3207,13 +3191,13 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="74" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B7" s="59"/>
       <c r="C7" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="58"/>
+      <c r="D7" s="75"/>
       <c r="E7" s="58"/>
       <c r="F7" s="58"/>
       <c r="G7" s="58"/>
@@ -3263,11 +3247,9 @@
     </row>
     <row r="12" spans="1:8" ht="53.25" customHeight="1">
       <c r="A12" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="80" t="s">
-        <v>29</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B12" s="77"/>
       <c r="C12" s="48"/>
       <c r="D12" s="48"/>
       <c r="E12" s="48"/>
@@ -3277,27 +3259,31 @@
     </row>
     <row r="13" spans="1:8" ht="15">
       <c r="A13" s="74" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="20"/>
+        <v>26</v>
+      </c>
+      <c r="B13" s="59"/>
       <c r="C13" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="55"/>
+      <c r="D13" s="73"/>
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
       <c r="G13" s="55"/>
       <c r="H13" s="55"/>
     </row>
-    <row r="14" spans="1:8" ht="15">
-      <c r="A14" s="56"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
+    <row r="14" spans="1:8">
+      <c r="A14" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="59"/>
+      <c r="C14" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="75"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:8" ht="15">
       <c r="A15" s="56"/>
@@ -3343,11 +3329,9 @@
     </row>
     <row r="19" spans="1:8" ht="63.75">
       <c r="A19" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>30</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B19" s="48"/>
       <c r="C19" s="48"/>
       <c r="D19" s="48"/>
       <c r="E19" s="48"/>
@@ -3357,7 +3341,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="74" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B20" s="59"/>
       <c r="C20" s="75" t="s">
@@ -3372,7 +3356,7 @@
     <row r="21" spans="1:8" ht="15">
       <c r="A21" s="74"/>
       <c r="B21" s="20"/>
-      <c r="C21" s="79"/>
+      <c r="C21" s="76"/>
       <c r="D21" s="55"/>
       <c r="E21" s="55"/>
       <c r="F21" s="55"/>
@@ -3423,11 +3407,9 @@
     </row>
     <row r="26" spans="1:8" ht="51">
       <c r="A26" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="80" t="s">
-        <v>32</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B26" s="77"/>
       <c r="C26" s="48"/>
       <c r="D26" s="48"/>
       <c r="E26" s="48"/>
@@ -3437,13 +3419,13 @@
     </row>
     <row r="27" spans="1:8" ht="15">
       <c r="A27" s="74" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="B27" s="20"/>
-      <c r="C27" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="55"/>
+      <c r="C27" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="76"/>
       <c r="E27" s="55"/>
       <c r="F27" s="55"/>
       <c r="G27" s="55"/>
@@ -3451,13 +3433,13 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="74" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="B28" s="59"/>
       <c r="C28" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="58"/>
+      <c r="D28" s="75"/>
       <c r="E28" s="58"/>
       <c r="F28" s="58"/>
       <c r="G28" s="58"/>
@@ -3507,11 +3489,9 @@
     </row>
     <row r="33" spans="1:8" ht="38.25">
       <c r="A33" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" s="48" t="s">
-        <v>30</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B33" s="48"/>
       <c r="C33" s="48"/>
       <c r="D33" s="48"/>
       <c r="E33" s="48"/>
@@ -3521,10 +3501,10 @@
     </row>
     <row r="34" spans="1:8" ht="15">
       <c r="A34" s="74" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B34" s="20"/>
-      <c r="C34" s="79" t="s">
+      <c r="C34" s="76" t="s">
         <v>17</v>
       </c>
       <c r="D34" s="55"/>
@@ -3536,7 +3516,7 @@
     <row r="35" spans="1:8" ht="15">
       <c r="A35" s="74"/>
       <c r="B35" s="20"/>
-      <c r="C35" s="79"/>
+      <c r="C35" s="76"/>
       <c r="D35" s="55"/>
       <c r="E35" s="55"/>
       <c r="F35" s="55"/>
@@ -3577,11 +3557,9 @@
     </row>
     <row r="39" spans="1:8" ht="38.25">
       <c r="A39" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" s="48" t="s">
-        <v>30</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B39" s="48"/>
       <c r="C39" s="48"/>
       <c r="D39" s="48"/>
       <c r="E39" s="48"/>
@@ -3591,45 +3569,45 @@
     </row>
     <row r="40" spans="1:8" ht="15">
       <c r="A40" s="74" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B40" s="20"/>
-      <c r="C40" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" s="55"/>
+      <c r="C40" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="76"/>
       <c r="E40" s="55"/>
       <c r="F40" s="55"/>
       <c r="G40" s="55"/>
       <c r="H40" s="55"/>
     </row>
-    <row r="41" spans="1:8" ht="15">
+    <row r="41" spans="1:8">
       <c r="A41" s="74" t="s">
-        <v>20</v>
-      </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="55"/>
-      <c r="E41" s="55"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="55"/>
+        <v>62</v>
+      </c>
+      <c r="B41" s="18"/>
+      <c r="C41" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="76"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="74" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
+        <v>33</v>
+      </c>
+      <c r="B42" s="59"/>
+      <c r="C42" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="75"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
     </row>
     <row r="43" spans="1:8" ht="15">
       <c r="A43" s="57"/>
@@ -3665,11 +3643,9 @@
     </row>
     <row r="46" spans="1:8" ht="51">
       <c r="A46" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B46" s="48" t="s">
-        <v>30</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B46" s="48"/>
       <c r="C46" s="48"/>
       <c r="D46" s="48"/>
       <c r="E46" s="48"/>
@@ -3679,10 +3655,10 @@
     </row>
     <row r="47" spans="1:8" ht="15">
       <c r="A47" s="74" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="B47" s="20"/>
-      <c r="C47" s="79" t="s">
+      <c r="C47" s="76" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="55"/>
@@ -3693,7 +3669,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="74" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="B48" s="59"/>
       <c r="C48" s="75" t="s">
@@ -3706,13 +3682,9 @@
       <c r="H48" s="58"/>
     </row>
     <row r="49" spans="1:8" ht="15">
-      <c r="A49" s="74" t="s">
-        <v>46</v>
-      </c>
+      <c r="A49" s="74"/>
       <c r="B49" s="20"/>
-      <c r="C49" s="79" t="s">
-        <v>17</v>
-      </c>
+      <c r="C49" s="76"/>
       <c r="D49" s="55"/>
       <c r="E49" s="55"/>
       <c r="F49" s="55"/>
@@ -3756,7 +3728,7 @@
         <v>5</v>
       </c>
       <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
+      <c r="C53" s="69"/>
       <c r="D53" s="27"/>
       <c r="E53" s="27"/>
       <c r="F53" s="27"/>
@@ -3768,7 +3740,7 @@
         <v>12</v>
       </c>
       <c r="B54" s="30"/>
-      <c r="C54" s="31"/>
+      <c r="C54" s="70"/>
       <c r="D54" s="31"/>
       <c r="E54" s="31"/>
       <c r="F54" s="31"/>
@@ -3789,11 +3761,9 @@
     </row>
     <row r="56" spans="1:8" ht="38.25">
       <c r="A56" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" s="37" t="s">
-        <v>30</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B56" s="37"/>
       <c r="C56" s="38"/>
       <c r="D56" s="38"/>
       <c r="E56" s="38"/>
@@ -3806,7 +3776,7 @@
         <v>21</v>
       </c>
       <c r="B57" s="20"/>
-      <c r="C57" s="79" t="s">
+      <c r="C57" s="76" t="s">
         <v>17</v>
       </c>
       <c r="D57" s="55"/>
@@ -3881,11 +3851,9 @@
     </row>
     <row r="64" spans="1:8" ht="63.75">
       <c r="A64" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="B64" s="44" t="s">
-        <v>30</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B64" s="44"/>
       <c r="C64" s="45"/>
       <c r="D64" s="45"/>
       <c r="E64" s="45"/>
@@ -3898,7 +3866,7 @@
         <v>22</v>
       </c>
       <c r="B65" s="20"/>
-      <c r="C65" s="79" t="s">
+      <c r="C65" s="76" t="s">
         <v>17</v>
       </c>
       <c r="D65" s="55"/>
@@ -3965,11 +3933,9 @@
     </row>
     <row r="71" spans="1:8" ht="26.25">
       <c r="A71" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="B71" s="46" t="s">
-        <v>30</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B71" s="46"/>
       <c r="C71" s="72"/>
       <c r="D71" s="47"/>
       <c r="E71" s="47"/>
@@ -4045,11 +4011,9 @@
     </row>
     <row r="78" spans="1:8" ht="51.75">
       <c r="A78" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="B78" s="47" t="s">
-        <v>30</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B78" s="47"/>
       <c r="C78" s="72"/>
       <c r="D78" s="47"/>
       <c r="E78" s="47"/>
@@ -4062,7 +4026,7 @@
         <v>23</v>
       </c>
       <c r="B79" s="20"/>
-      <c r="C79" s="79" t="s">
+      <c r="C79" s="76" t="s">
         <v>17</v>
       </c>
       <c r="D79" s="55"/>
@@ -4073,7 +4037,7 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="74" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B80" s="59"/>
       <c r="C80" s="73" t="s">
@@ -4086,9 +4050,13 @@
       <c r="H80" s="58"/>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="19"/>
-      <c r="B81" s="18"/>
-      <c r="C81" s="71"/>
+      <c r="A81" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B81" s="20"/>
+      <c r="C81" s="76" t="s">
+        <v>17</v>
+      </c>
       <c r="D81" s="18"/>
       <c r="E81" s="18"/>
       <c r="F81" s="18"/>
@@ -4096,9 +4064,13 @@
       <c r="H81" s="18"/>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="19"/>
+      <c r="A82" s="74" t="s">
+        <v>62</v>
+      </c>
       <c r="B82" s="18"/>
-      <c r="C82" s="71"/>
+      <c r="C82" s="76" t="s">
+        <v>17</v>
+      </c>
       <c r="D82" s="18"/>
       <c r="E82" s="18"/>
       <c r="F82" s="18"/>
@@ -4129,11 +4101,9 @@
     </row>
     <row r="85" spans="1:8" ht="64.5">
       <c r="A85" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="B85" s="37" t="s">
-        <v>30</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B85" s="37"/>
       <c r="C85" s="72"/>
       <c r="D85" s="47"/>
       <c r="E85" s="47"/>
@@ -4143,7 +4113,7 @@
     </row>
     <row r="86" spans="1:8">
       <c r="A86" s="74" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="B86" s="59"/>
       <c r="C86" s="73" t="s">
@@ -4157,10 +4127,10 @@
     </row>
     <row r="87" spans="1:8" ht="15">
       <c r="A87" s="74" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B87" s="20"/>
-      <c r="C87" s="79" t="s">
+      <c r="C87" s="76" t="s">
         <v>17</v>
       </c>
       <c r="D87" s="55"/>
@@ -4213,11 +4183,9 @@
     </row>
     <row r="92" spans="1:8" ht="51.75">
       <c r="A92" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="B92" s="47" t="s">
-        <v>30</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B92" s="47"/>
       <c r="C92" s="72"/>
       <c r="D92" s="47"/>
       <c r="E92" s="47"/>
@@ -4227,10 +4195,10 @@
     </row>
     <row r="93" spans="1:8" ht="15">
       <c r="A93" s="74" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B93" s="20"/>
-      <c r="C93" s="79" t="s">
+      <c r="C93" s="76" t="s">
         <v>17</v>
       </c>
       <c r="D93" s="55"/>
@@ -4241,7 +4209,7 @@
     </row>
     <row r="94" spans="1:8">
       <c r="A94" s="74" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B94" s="59"/>
       <c r="C94" s="73" t="s">
@@ -4297,11 +4265,9 @@
     </row>
     <row r="99" spans="1:8" ht="64.5">
       <c r="A99" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="B99" s="37" t="s">
-        <v>30</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B99" s="37"/>
       <c r="C99" s="72"/>
       <c r="D99" s="47"/>
       <c r="E99" s="47"/>
@@ -4311,10 +4277,10 @@
     </row>
     <row r="100" spans="1:8" ht="15">
       <c r="A100" s="74" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B100" s="20"/>
-      <c r="C100" s="79" t="s">
+      <c r="C100" s="76" t="s">
         <v>17</v>
       </c>
       <c r="D100" s="55"/>
@@ -4325,7 +4291,7 @@
     </row>
     <row r="101" spans="1:8">
       <c r="A101" s="74" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B101" s="59"/>
       <c r="C101" s="75" t="s">
@@ -4381,11 +4347,9 @@
     </row>
     <row r="106" spans="1:8" ht="69.75" customHeight="1">
       <c r="A106" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="B106" s="37" t="s">
-        <v>36</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B106" s="37"/>
       <c r="C106" s="72"/>
       <c r="D106" s="47"/>
       <c r="E106" s="47"/>
@@ -4395,10 +4359,10 @@
     </row>
     <row r="107" spans="1:8" ht="15">
       <c r="A107" s="74" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="B107" s="20"/>
-      <c r="C107" s="79" t="s">
+      <c r="C107" s="76" t="s">
         <v>17</v>
       </c>
       <c r="D107" s="55"/>
@@ -4408,9 +4372,13 @@
       <c r="H107" s="55"/>
     </row>
     <row r="108" spans="1:8">
-      <c r="A108" s="19"/>
-      <c r="B108" s="18"/>
-      <c r="C108" s="71"/>
+      <c r="A108" s="74" t="s">
+        <v>67</v>
+      </c>
+      <c r="B108" s="20"/>
+      <c r="C108" s="76" t="s">
+        <v>17</v>
+      </c>
       <c r="D108" s="18"/>
       <c r="E108" s="18"/>
       <c r="F108" s="18"/>
@@ -4461,11 +4429,9 @@
     </row>
     <row r="113" spans="1:8" ht="64.5">
       <c r="A113" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="B113" s="47" t="s">
-        <v>30</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B113" s="47"/>
       <c r="C113" s="72"/>
       <c r="D113" s="47"/>
       <c r="E113" s="47"/>
@@ -4475,10 +4441,10 @@
     </row>
     <row r="114" spans="1:8">
       <c r="A114" s="74" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B114" s="18"/>
-      <c r="C114" s="79" t="s">
+      <c r="C114" s="76" t="s">
         <v>17</v>
       </c>
       <c r="D114" s="18"/>
@@ -4488,9 +4454,13 @@
       <c r="H114" s="18"/>
     </row>
     <row r="115" spans="1:8">
-      <c r="A115" s="19"/>
-      <c r="B115" s="18"/>
-      <c r="C115" s="71"/>
+      <c r="A115" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B115" s="20"/>
+      <c r="C115" s="76" t="s">
+        <v>17</v>
+      </c>
       <c r="D115" s="18"/>
       <c r="E115" s="18"/>
       <c r="F115" s="18"/>
@@ -4498,9 +4468,13 @@
       <c r="H115" s="18"/>
     </row>
     <row r="116" spans="1:8">
-      <c r="A116" s="19"/>
+      <c r="A116" s="74" t="s">
+        <v>62</v>
+      </c>
       <c r="B116" s="18"/>
-      <c r="C116" s="71"/>
+      <c r="C116" s="76" t="s">
+        <v>17</v>
+      </c>
       <c r="D116" s="18"/>
       <c r="E116" s="18"/>
       <c r="F116" s="18"/>
@@ -4541,11 +4515,9 @@
     </row>
     <row r="120" spans="1:8" ht="64.5">
       <c r="A120" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="B120" s="47" t="s">
-        <v>36</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B120" s="47"/>
       <c r="C120" s="72"/>
       <c r="D120" s="47"/>
       <c r="E120" s="47"/>
@@ -4555,7 +4527,7 @@
     </row>
     <row r="121" spans="1:8">
       <c r="A121" s="74" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B121" s="59"/>
       <c r="C121" s="73" t="s">
@@ -4569,10 +4541,10 @@
     </row>
     <row r="122" spans="1:8">
       <c r="A122" s="74" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B122" s="18"/>
-      <c r="C122" s="79" t="s">
+      <c r="C122" s="76" t="s">
         <v>17</v>
       </c>
       <c r="D122" s="18"/>
@@ -4583,10 +4555,10 @@
     </row>
     <row r="123" spans="1:8" ht="15">
       <c r="A123" s="74" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B123" s="20"/>
-      <c r="C123" s="79" t="s">
+      <c r="C123" s="76" t="s">
         <v>17</v>
       </c>
       <c r="D123" s="55"/>
@@ -4596,9 +4568,13 @@
       <c r="H123" s="55"/>
     </row>
     <row r="124" spans="1:8">
-      <c r="A124" s="19"/>
+      <c r="A124" s="74" t="s">
+        <v>62</v>
+      </c>
       <c r="B124" s="18"/>
-      <c r="C124" s="71"/>
+      <c r="C124" s="76" t="s">
+        <v>17</v>
+      </c>
       <c r="D124" s="18"/>
       <c r="E124" s="18"/>
       <c r="F124" s="18"/>
@@ -4634,7 +4610,7 @@
       <c r="B128" s="5"/>
     </row>
     <row r="129" spans="1:2" customFormat="1">
-      <c r="A129" s="81"/>
+      <c r="A129" s="78"/>
       <c r="B129" s="5"/>
     </row>
     <row r="130" spans="1:2" customFormat="1">
@@ -4700,39 +4676,45 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C13" r:id="rId1"/>
-    <hyperlink ref="C7" r:id="rId2"/>
-    <hyperlink ref="C6" r:id="rId3"/>
-    <hyperlink ref="C28" r:id="rId4"/>
-    <hyperlink ref="C34" r:id="rId5"/>
-    <hyperlink ref="C41" r:id="rId6"/>
-    <hyperlink ref="C57" r:id="rId7"/>
-    <hyperlink ref="C65" r:id="rId8"/>
-    <hyperlink ref="C72" r:id="rId9"/>
-    <hyperlink ref="C79" r:id="rId10"/>
-    <hyperlink ref="C66" r:id="rId11"/>
-    <hyperlink ref="C80" r:id="rId12"/>
-    <hyperlink ref="C86" r:id="rId13"/>
-    <hyperlink ref="C87" r:id="rId14"/>
-    <hyperlink ref="C93" r:id="rId15"/>
-    <hyperlink ref="C94" r:id="rId16"/>
-    <hyperlink ref="C100" r:id="rId17"/>
-    <hyperlink ref="C101" r:id="rId18"/>
-    <hyperlink ref="C107" r:id="rId19"/>
-    <hyperlink ref="C114" r:id="rId20"/>
-    <hyperlink ref="C121" r:id="rId21"/>
-    <hyperlink ref="C122" r:id="rId22"/>
-    <hyperlink ref="C27" r:id="rId23"/>
-    <hyperlink ref="C48" r:id="rId24"/>
-    <hyperlink ref="C47" r:id="rId25"/>
-    <hyperlink ref="C123" r:id="rId26"/>
-    <hyperlink ref="C42" r:id="rId27"/>
-    <hyperlink ref="C20" r:id="rId28"/>
-    <hyperlink ref="C40" r:id="rId29"/>
-    <hyperlink ref="C49" r:id="rId30"/>
+    <hyperlink ref="C34" r:id="rId1"/>
+    <hyperlink ref="C48" r:id="rId2"/>
+    <hyperlink ref="C47" r:id="rId3"/>
+    <hyperlink ref="C20" r:id="rId4"/>
+    <hyperlink ref="C57" r:id="rId5"/>
+    <hyperlink ref="C108" r:id="rId6"/>
+    <hyperlink ref="C114" r:id="rId7"/>
+    <hyperlink ref="C123" r:id="rId8"/>
+    <hyperlink ref="C81" r:id="rId9"/>
+    <hyperlink ref="C82" r:id="rId10"/>
+    <hyperlink ref="C115" r:id="rId11"/>
+    <hyperlink ref="C116" r:id="rId12"/>
+    <hyperlink ref="C124" r:id="rId13"/>
+    <hyperlink ref="C66" r:id="rId14"/>
+    <hyperlink ref="C72" r:id="rId15"/>
+    <hyperlink ref="C80" r:id="rId16"/>
+    <hyperlink ref="C86" r:id="rId17"/>
+    <hyperlink ref="C94" r:id="rId18"/>
+    <hyperlink ref="C121" r:id="rId19"/>
+    <hyperlink ref="C101" r:id="rId20"/>
+    <hyperlink ref="C65" r:id="rId21"/>
+    <hyperlink ref="C79" r:id="rId22"/>
+    <hyperlink ref="C87" r:id="rId23"/>
+    <hyperlink ref="C93" r:id="rId24"/>
+    <hyperlink ref="C100" r:id="rId25"/>
+    <hyperlink ref="C107" r:id="rId26"/>
+    <hyperlink ref="C122" r:id="rId27"/>
+    <hyperlink ref="C6" r:id="rId28"/>
+    <hyperlink ref="C7" r:id="rId29"/>
+    <hyperlink ref="C13" r:id="rId30"/>
+    <hyperlink ref="C14" r:id="rId31"/>
+    <hyperlink ref="C28" r:id="rId32"/>
+    <hyperlink ref="C27" r:id="rId33"/>
+    <hyperlink ref="C40" r:id="rId34"/>
+    <hyperlink ref="C42" r:id="rId35"/>
+    <hyperlink ref="C41" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.49212598499999999" footer="0.49212598499999999"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId37"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>